<commit_message>
Added src and docs folders...added detailed moldels of hardware components, added beginning of  a literature review and a completed bill of materials.
there should be everything in here required for someone to replicate the rotoforge project. its not perfectly organized yet so I am happy to provide some help to the intrepid explorers interested in working with me on it.
</commit_message>
<xml_diff>
--- a/billofmaterials.xlsx
+++ b/billofmaterials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Unit-005\Documents\Rotoforge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472271A6-C090-426B-A0A0-D84E2547E5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A8F72C-52D6-4AD0-AA98-F90FAB9C9228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{25EE2794-6DB4-40A8-8AE6-DE6B297337A8}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{25EE2794-6DB4-40A8-8AE6-DE6B297337A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
   <si>
     <t>Item</t>
   </si>
@@ -68,9 +68,6 @@
     <t>XING E-Flight</t>
   </si>
   <si>
-    <t>Aluminum angle 1"*1" *L</t>
-  </si>
-  <si>
     <t>M3 drill bit</t>
   </si>
   <si>
@@ -255,6 +252,45 @@
   </si>
   <si>
     <t>7mm M2 HSS tool steel rod</t>
+  </si>
+  <si>
+    <t>Bannana clips</t>
+  </si>
+  <si>
+    <t>ESC motor speed controller</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/RC-Brushless-Electric-Controller-bullet/dp/B071GRSFBD/ref=sr_1_1?keywords=ESC&amp;qid=1675127368&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>Speed controller for BLDC motor</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Plated-Screw-Banana-Plugs-16-Pack/dp/B07SSP3KFB/ref=sr_1_14?crid=3VQ8PN37MZ6H8&amp;keywords=screw+terminal+banana+plugs&amp;qid=1675127515&amp;sprefix=screw+terminal+banan+plugs%2Caps%2C138&amp;sr=8-14</t>
+  </si>
+  <si>
+    <t>plugs from BLDC to ESC</t>
+  </si>
+  <si>
+    <t>1.8 mm dill bit</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Mtsooning-1-8mm-Straight-Electrical-Drilling/dp/B071G2HLX7/ref=sr_1_3?crid=1MV4UUUOK3X85&amp;keywords=1.8+mm+drill+bit&amp;qid=1675127999&amp;sprefix=1.8+mm+drill+b%2Caps%2C360&amp;sr=8-3</t>
+  </si>
+  <si>
+    <t>drill bit for drilling the PEEK screw</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/FullerKreg-M5-0-8-Stainless-Steel-Acorn/dp/B07DB4ZR3F/ref=sr_1_1?crid=3LAM0LFPL1BVY&amp;keywords=m5%2Bstainless%2Bacorn%2Bnuts&amp;qid=1675128694&amp;sprefix=m5%2Bstainless%2Bacorn%2Bnut%2Caps%2C161&amp;sr=8-1&amp;th=1</t>
+  </si>
+  <si>
+    <t>Blanks for nozzle/tool/die fabrication</t>
+  </si>
+  <si>
+    <t>M5 Stainless steel acorn nuts</t>
+  </si>
+  <si>
+    <t>Aluminum angle 1"*1" *1/8" *L</t>
   </si>
 </sst>
 </file>
@@ -617,23 +653,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA526714-29D0-411C-BFE9-D267D53463AB}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="148.77734375" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="148.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -664,19 +700,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>190</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -690,237 +726,237 @@
         <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
       </c>
       <c r="D8">
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
       </c>
       <c r="D9">
         <v>8.49</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <f>0.7*B10</f>
         <v>0.7</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
       </c>
       <c r="D11">
         <f>1.2*B11</f>
         <v>1.2</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>13.39</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>18.59</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>22</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
       </c>
       <c r="D14">
         <v>11.99</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -933,119 +969,199 @@
         <v>0.36</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16">
         <v>8.49</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17">
         <v>14.57</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>23.57</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>65</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>66</v>
       </c>
       <c r="D19">
         <v>1.9</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20">
         <v>6.59</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
       <c r="D21">
-        <f>SUM(D2:D20)</f>
-        <v>427.83999999999992</v>
+        <v>10.87</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>77</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="E22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>5.99</v>
+      </c>
+      <c r="E23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f>SUM(D2:D24)</f>
+        <v>469.68999999999994</v>
+      </c>
+      <c r="E25" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1068,6 +1184,10 @@
     <hyperlink ref="G18" r:id="rId16" xr:uid="{5D05E51D-4908-4EC7-9344-A5ED181420EB}"/>
     <hyperlink ref="G19" r:id="rId17" xr:uid="{1093EC71-AD94-47E7-A2CD-A6C09B050755}"/>
     <hyperlink ref="G20" r:id="rId18" xr:uid="{980517EA-698E-45CE-80B4-E7A90D6DBCA1}"/>
+    <hyperlink ref="G22" r:id="rId19" xr:uid="{D30124FA-7152-4FB2-9696-36ACB8926330}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{B765AFAC-8C4A-4CE7-843F-65EA824E145E}"/>
+    <hyperlink ref="G23" r:id="rId21" xr:uid="{0F19DA50-0A7F-421E-9381-E3B5F9CE6B2E}"/>
+    <hyperlink ref="G24" r:id="rId22" xr:uid="{6370200D-A282-42E4-8BF4-45AC4BC45AE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>